<commit_message>
Anadiendo requisito añadir adisionales
</commit_message>
<xml_diff>
--- a/Desarrollo/GSC/Gestion/Cronograma.xlsx
+++ b/Desarrollo/GSC/Gestion/Cronograma.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROYECTO\FisiDev-Solutions\Desarrollo\GSC\Gestion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Gestión de la configuración\FisiDev-Solutions\Desarrollo\GSC\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DCBA43-79AA-444B-919A-DE5D6590057C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRONOGRAMA" sheetId="1" r:id="rId1"/>
@@ -224,8 +225,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -655,7 +656,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="CRONOGRAMA-style" pivot="0" count="3">
+    <tableStyle name="CRONOGRAMA-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
@@ -673,15 +674,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="CRONOGRAMA_DE_ACTIVIDADES" displayName="CRONOGRAMA_DE_ACTIVIDADES" ref="A1:G18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="CRONOGRAMA_DE_ACTIVIDADES" displayName="CRONOGRAMA_DE_ACTIVIDADES" ref="A1:G18">
   <tableColumns count="7">
-    <tableColumn id="1" name="Tarea"/>
-    <tableColumn id="2" name="ARTEFACTO"/>
-    <tableColumn id="3" name="NOMENCLATURA"/>
-    <tableColumn id="4" name="ROL"/>
-    <tableColumn id="5" name="INICIO"/>
-    <tableColumn id="6" name="FIN"/>
-    <tableColumn id="7" name="ESTADO"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tarea"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ARTEFACTO"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="NOMENCLATURA"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ROL"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="INICIO"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="FIN"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="ESTADO"/>
   </tableColumns>
   <tableStyleInfo name="CRONOGRAMA-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -884,7 +885,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -892,21 +893,21 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" customWidth="1"/>
+    <col min="1" max="1" width="44.5546875" customWidth="1"/>
+    <col min="2" max="2" width="43.44140625" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -929,7 +930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -952,7 +953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
@@ -972,11 +973,11 @@
         <v>45750</v>
       </c>
       <c r="G3" s="35">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -996,10 +997,10 @@
         <v>45757</v>
       </c>
       <c r="G4" s="34">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>17</v>
       </c>
@@ -1019,10 +1020,10 @@
         <v>45764</v>
       </c>
       <c r="G5" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
@@ -1045,7 +1046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>24</v>
       </c>
@@ -1066,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>25</v>
       </c>
@@ -1089,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28" t="s">
         <v>29</v>
       </c>
@@ -1112,7 +1113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>33</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>37</v>
       </c>
@@ -1158,7 +1159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>40</v>
       </c>
@@ -1179,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>41</v>
       </c>
@@ -1202,7 +1203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>45</v>
       </c>
@@ -1225,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>49</v>
       </c>
@@ -1248,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>53</v>
       </c>
@@ -1271,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>57</v>
       </c>
@@ -1294,7 +1295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>61</v>
       </c>
@@ -1319,17 +1320,17 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" sqref="G2:G18">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G18" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Sin comenzar,En curso,Bloqueado,Completado"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:F18">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:F18" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>OR(NOT(ISERROR(DATEVALUE(E2))), AND(ISNUMBER(E2), LEFT(CELL("format", E2))="D"))</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:D18"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A2:D18" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C6" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>